<commit_message>
Update expected output for negative UI test case
</commit_message>
<xml_diff>
--- a/IT23328952 - Test cases new.xlsx
+++ b/IT23328952 - Test cases new.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="534">
   <si>
     <t xml:space="preserve">Note: </t>
   </si>
@@ -4396,6 +4396,94 @@
         <charset val="134"/>
       </rPr>
       <t>Real-time output update behavior</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Neg_UI_0001 </t>
+  </si>
+  <si>
+    <t>Clear/reset functionality not working properly</t>
+  </si>
+  <si>
+    <t>Test clearing the input field after entering: mama gedhara yanavaa</t>
+  </si>
+  <si>
+    <t>Both input and output fields should be completely cleared when clear button is clicked or input is manually deleted</t>
+  </si>
+  <si>
+    <t>UI clear function fails to reset output field, or residual text remains. User must manually refresh page to clear completely. Affects usability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usability flow (input clearing)
+</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Simple sentence</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve">S (≤30 characters) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="2"/>
+      </rPr>
+      <t>Error handling / input validation</t>
     </r>
   </si>
   <si>
@@ -10155,6 +10243,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -10303,16 +10397,25 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="7"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <charset val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <i/>
@@ -10322,8 +10425,21 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
@@ -10346,34 +10462,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
@@ -10751,13 +10839,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -10766,119 +10851,122 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -11006,6 +11094,21 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -11326,10 +11429,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M153"/>
+  <dimension ref="A1:M157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150:B153"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="I157" sqref="I157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="49.95" customHeight="1"/>
@@ -14081,8 +14184,76 @@
         <v>301</v>
       </c>
     </row>
+    <row r="154" customHeight="1" spans="1:9">
+      <c r="A154" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="B154" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="C154" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D154" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="E154" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="F154" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="G154" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="H154" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="I154" s="48" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="155" customHeight="1" spans="1:9">
+      <c r="A155" s="25"/>
+      <c r="B155" s="24"/>
+      <c r="C155" s="24"/>
+      <c r="D155" s="33"/>
+      <c r="E155" s="33"/>
+      <c r="F155" s="33"/>
+      <c r="G155" s="24"/>
+      <c r="H155" s="45"/>
+      <c r="I155" s="27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="156" customHeight="1" spans="1:9">
+      <c r="A156" s="25"/>
+      <c r="B156" s="24"/>
+      <c r="C156" s="24"/>
+      <c r="D156" s="33"/>
+      <c r="E156" s="33"/>
+      <c r="F156" s="33"/>
+      <c r="G156" s="24"/>
+      <c r="H156" s="46"/>
+      <c r="I156" s="27" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="157" customHeight="1" spans="1:9">
+      <c r="A157" s="25"/>
+      <c r="B157" s="24"/>
+      <c r="C157" s="24"/>
+      <c r="D157" s="33"/>
+      <c r="E157" s="33"/>
+      <c r="F157" s="34"/>
+      <c r="G157" s="24"/>
+      <c r="H157" s="47"/>
+      <c r="I157" s="27" t="s">
+        <v>310</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="263">
+  <mergeCells count="271">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:I3"/>
@@ -14124,6 +14295,7 @@
     <mergeCell ref="A142:A145"/>
     <mergeCell ref="A146:A149"/>
     <mergeCell ref="A150:A153"/>
+    <mergeCell ref="A154:A157"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
@@ -14161,6 +14333,7 @@
     <mergeCell ref="B142:B145"/>
     <mergeCell ref="B146:B149"/>
     <mergeCell ref="B150:B153"/>
+    <mergeCell ref="B154:B157"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="C14:C17"/>
@@ -14198,6 +14371,7 @@
     <mergeCell ref="C142:C145"/>
     <mergeCell ref="C146:C149"/>
     <mergeCell ref="C150:C153"/>
+    <mergeCell ref="C154:C157"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="D10:D13"/>
     <mergeCell ref="D14:D17"/>
@@ -14235,6 +14409,7 @@
     <mergeCell ref="D142:D145"/>
     <mergeCell ref="D146:D149"/>
     <mergeCell ref="D150:D153"/>
+    <mergeCell ref="D154:D157"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="E10:E13"/>
     <mergeCell ref="E14:E17"/>
@@ -14272,6 +14447,7 @@
     <mergeCell ref="E142:E145"/>
     <mergeCell ref="E146:E149"/>
     <mergeCell ref="E150:E153"/>
+    <mergeCell ref="E154:E157"/>
     <mergeCell ref="F6:F9"/>
     <mergeCell ref="F10:F13"/>
     <mergeCell ref="F14:F17"/>
@@ -14309,6 +14485,7 @@
     <mergeCell ref="F142:F145"/>
     <mergeCell ref="F146:F149"/>
     <mergeCell ref="F150:F153"/>
+    <mergeCell ref="F154:F157"/>
     <mergeCell ref="G6:G9"/>
     <mergeCell ref="G10:G13"/>
     <mergeCell ref="G14:G17"/>
@@ -14346,6 +14523,8 @@
     <mergeCell ref="G142:G145"/>
     <mergeCell ref="G146:G149"/>
     <mergeCell ref="G150:G153"/>
+    <mergeCell ref="G154:G157"/>
+    <mergeCell ref="H154:H156"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D134" r:id="rId1" display="https://www.swissgear.com " tooltip="https://www.swissgear.com "/>
@@ -14372,27 +14551,27 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:1">
@@ -14400,22 +14579,22 @@
     </row>
     <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
       <c r="A8" s="2" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -14440,92 +14619,92 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="10" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="11" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="11" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="11" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="10" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="11" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="11" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="11" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="10" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="11" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="11" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="11" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="9" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="10" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="11" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="11" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="11" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -14533,97 +14712,97 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="10" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="11" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="11" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="11" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="11" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="9" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="10" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="11" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="11" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="11" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="10" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="11" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="11" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="11" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="9" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="10" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="11" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="11" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="11" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
     </row>
     <row r="47" spans="1:1">
@@ -14631,117 +14810,117 @@
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="10" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="11" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="11" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="11" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="10" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="11" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="11" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="11" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="9" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="10" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="11" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="11" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="11" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="10" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="11" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="11" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="11" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="9" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="11" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="11" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="11" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="11" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="11" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
     </row>
     <row r="75" spans="1:1">
@@ -14752,107 +14931,107 @@
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="9" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="11" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="11" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="11" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="11" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="11" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="11" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="9" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="10" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="11" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="11" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="11" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="10" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="11" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="11" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="11" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="9" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="11" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="11" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="11" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="11" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
     </row>
     <row r="102" spans="1:1">
@@ -14863,117 +15042,117 @@
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="9" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="10" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="11" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="11" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="10" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="11" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="11" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="10" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="11" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="11" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="9" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="11" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="11" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="11" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" s="9" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="10" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" s="11" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="11" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" s="11" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="10" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" s="11" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="11" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="11" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="131" spans="1:1">
@@ -14984,102 +15163,102 @@
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="9" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" s="11" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="11" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" s="11" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" s="11" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" s="9" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="11" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" s="11" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="11" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" s="11" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="11" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="11" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" s="9" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" s="11" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" s="11" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" s="11" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" s="11" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" s="11" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" s="11" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" s="11" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
     </row>
     <row r="157" spans="1:1">
@@ -15090,162 +15269,162 @@
     </row>
     <row r="159" spans="1:1">
       <c r="A159" s="9" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" s="11" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" s="11" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" s="11" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" s="11" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" s="11" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" s="11" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" s="11" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" s="9" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" s="11" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" s="11" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" s="11" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" s="11" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" s="9" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" s="10" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" s="11" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" s="11" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" s="10" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" s="13" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" s="13" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" s="10" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" s="13" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" s="13" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" s="13" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" s="10" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" s="13" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" s="13" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" s="13" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" s="9" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" s="10" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" s="11" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" s="11" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
     </row>
     <row r="197" spans="1:1">
@@ -15253,72 +15432,72 @@
     </row>
     <row r="198" spans="1:1">
       <c r="A198" s="10" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" s="13" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" s="12" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" s="14" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" s="12" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" s="10" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
     </row>
     <row r="204" ht="27.6" spans="1:1">
       <c r="A204" s="15" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" s="9" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" s="11" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" s="11" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" s="11" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" s="11" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" s="11" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" s="11" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -15343,27 +15522,27 @@
   <sheetData>
     <row r="1" ht="16.8" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>482</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -15371,202 +15550,202 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="4" t="s">
-        <v>485</v>
+        <v>494</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="5" t="s">
-        <v>486</v>
+        <v>495</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="6" t="s">
-        <v>487</v>
+        <v>496</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="6" t="s">
-        <v>488</v>
+        <v>497</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="6" t="s">
-        <v>489</v>
+        <v>498</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="6" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="6" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="6" t="s">
-        <v>492</v>
+        <v>501</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="6" t="s">
-        <v>493</v>
+        <v>502</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="6" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="6" t="s">
-        <v>495</v>
+        <v>504</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="6" t="s">
-        <v>496</v>
+        <v>505</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>497</v>
+        <v>506</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="6" t="s">
-        <v>498</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="6" t="s">
-        <v>499</v>
+        <v>508</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="6" t="s">
-        <v>500</v>
+        <v>509</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="6" t="s">
-        <v>501</v>
+        <v>510</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="6" t="s">
-        <v>502</v>
+        <v>511</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="6" t="s">
-        <v>503</v>
+        <v>512</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="6" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="6" t="s">
-        <v>505</v>
+        <v>514</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="6" t="s">
-        <v>506</v>
+        <v>515</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
-        <v>507</v>
+        <v>516</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="6" t="s">
-        <v>508</v>
+        <v>517</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="6" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="6" t="s">
-        <v>510</v>
+        <v>519</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
-        <v>511</v>
+        <v>520</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="6" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="7" t="s">
-        <v>513</v>
+        <v>522</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="8" t="s">
-        <v>514</v>
+        <v>523</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="8" t="s">
-        <v>515</v>
+        <v>524</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="8" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="8" t="s">
-        <v>517</v>
+        <v>526</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="6" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="7" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="8" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="8" t="s">
-        <v>521</v>
+        <v>530</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="6" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="6" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="6" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>